<commit_message>
edit clickEvent() +add clicked list to tree
</commit_message>
<xml_diff>
--- a/excelhere/room_three.xlsx
+++ b/excelhere/room_three.xlsx
@@ -442,21 +442,9 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>33</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
+      <c r="A1" t="inlineStr"/>
+      <c r="B1" t="inlineStr"/>
+      <c r="C1" t="inlineStr"/>
       <c r="D1" t="inlineStr">
         <is>
           <t>3</t>

</xml_diff>